<commit_message>
Stok kartları ayrıştırılmasına başlandı
</commit_message>
<xml_diff>
--- a/assets/SİPARİŞLER/Siparis formu - MER TEKNİK (YENİ).xlsx
+++ b/assets/SİPARİŞLER/Siparis formu - MER TEKNİK (YENİ).xlsx
@@ -5,24 +5,26 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yapisan Depo\Desktop\SİPARİŞLER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\deppo\assets\SİPARİŞLER\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="SİPARİŞ FORMU" sheetId="3" r:id="rId1"/>
+    <sheet name="SİPARİŞ FORMU (2)" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'SİPARİŞ FORMU'!$A$1:$J$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'SİPARİŞ FORMU (2)'!$A$1:$J$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>MEHMET KUYUCAK</t>
   </si>
@@ -187,6 +189,12 @@
   </si>
   <si>
     <t>TEMİZLİK SÜPÜRGESİ</t>
+  </si>
+  <si>
+    <t>M10X40 IMBUS CIVATA</t>
+  </si>
+  <si>
+    <t>M12 KLİPSLİ ÇELİK DÜBEL</t>
   </si>
 </sst>
 </file>
@@ -793,7 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,6 +896,153 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -900,6 +1055,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -956,171 +1132,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1146,6 +1157,158 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>473448</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="28575"/>
+          <a:ext cx="1845048" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>174249</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1830550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 659">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="174249" y="282949"/>
+          <a:ext cx="3027901" cy="770405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1590,7 +1753,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
@@ -1615,12 +1778,12 @@
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="22"/>
@@ -1662,34 +1825,34 @@
       <c r="A5" s="22"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="66" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
+      <c r="A7" s="103"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="23"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
@@ -1699,18 +1862,18 @@
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A8" s="47"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="108"/>
     </row>
     <row r="9" spans="1:10" ht="22.5" customHeight="1">
       <c r="A9" s="28"/>
@@ -1719,102 +1882,102 @@
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="53" t="s">
+      <c r="H9" s="106"/>
+      <c r="I9" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="54"/>
+      <c r="J9" s="110"/>
     </row>
     <row r="10" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="114"/>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="61" t="s">
+      <c r="B11" s="116"/>
+      <c r="C11" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="118"/>
     </row>
     <row r="12" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="90"/>
+      <c r="C12" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="92"/>
     </row>
     <row r="13" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="92"/>
     </row>
     <row r="14" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="92"/>
     </row>
     <row r="15" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="92"/>
     </row>
     <row r="16" spans="1:10" ht="22.5">
       <c r="A16" s="4"/>
@@ -1829,32 +1992,32 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="65"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="95"/>
     </row>
     <row r="18" spans="1:15" ht="22.5">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="99"/>
       <c r="G18" s="25" t="s">
         <v>3</v>
       </c>
@@ -1869,16 +2032,16 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A19" s="70">
+      <c r="A19" s="74">
         <v>1</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="38"/>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="73"/>
-      <c r="F19" s="71"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="75"/>
       <c r="G19" s="38">
         <v>2</v>
       </c>
@@ -1892,21 +2055,21 @@
         <f>G19*I19</f>
         <v>0</v>
       </c>
-      <c r="M19" s="117"/>
-      <c r="N19" s="117"/>
-      <c r="O19" s="117"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
     </row>
     <row r="20" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A20" s="70">
+      <c r="A20" s="74">
         <v>2</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="38"/>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="73"/>
-      <c r="F20" s="71"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="75"/>
       <c r="G20" s="38">
         <v>48</v>
       </c>
@@ -1920,21 +2083,21 @@
         <f t="shared" ref="J20:J31" si="0">G20*I20</f>
         <v>0</v>
       </c>
-      <c r="M20" s="117"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="117"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A21" s="70">
+      <c r="A21" s="74">
         <v>3</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="38"/>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="73"/>
-      <c r="F21" s="71"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="75"/>
       <c r="G21" s="38">
         <v>10</v>
       </c>
@@ -1948,21 +2111,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M21" s="117"/>
-      <c r="N21" s="117"/>
-      <c r="O21" s="117"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
     </row>
     <row r="22" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A22" s="70">
+      <c r="A22" s="74">
         <v>4</v>
       </c>
-      <c r="B22" s="71"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="38"/>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="73"/>
-      <c r="F22" s="71"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="75"/>
       <c r="G22" s="38">
         <v>10</v>
       </c>
@@ -1976,21 +2139,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M22" s="117"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="117"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
     </row>
     <row r="23" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A23" s="70">
+      <c r="A23" s="74">
         <v>5</v>
       </c>
-      <c r="B23" s="71"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="38"/>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="73"/>
-      <c r="F23" s="71"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="75"/>
       <c r="G23" s="38">
         <v>5</v>
       </c>
@@ -2004,23 +2167,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M23" s="117"/>
-      <c r="N23" s="117"/>
-      <c r="O23" s="117"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
     </row>
     <row r="24" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A24" s="70">
+      <c r="A24" s="74">
         <v>6</v>
       </c>
-      <c r="B24" s="71"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="72" t="s">
+      <c r="D24" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="73"/>
-      <c r="F24" s="71"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="75"/>
       <c r="G24" s="38">
         <v>1</v>
       </c>
@@ -2034,23 +2197,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
     </row>
     <row r="25" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A25" s="70">
+      <c r="A25" s="74">
         <v>7</v>
       </c>
-      <c r="B25" s="71"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D25" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="73"/>
-      <c r="F25" s="71"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="75"/>
       <c r="G25" s="38">
         <v>1</v>
       </c>
@@ -2064,23 +2227,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M25" s="117"/>
-      <c r="N25" s="117"/>
-      <c r="O25" s="117"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
     </row>
     <row r="26" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A26" s="70">
+      <c r="A26" s="74">
         <v>8</v>
       </c>
-      <c r="B26" s="71"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="71"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="75"/>
       <c r="G26" s="38">
         <v>1</v>
       </c>
@@ -2094,23 +2257,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M26" s="117"/>
-      <c r="N26" s="117"/>
-      <c r="O26" s="117"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
     </row>
     <row r="27" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A27" s="70">
+      <c r="A27" s="74">
         <v>9</v>
       </c>
-      <c r="B27" s="71"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="73"/>
-      <c r="F27" s="71"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="75"/>
       <c r="G27" s="38">
         <v>1</v>
       </c>
@@ -2124,23 +2287,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M27" s="117"/>
-      <c r="N27" s="117"/>
-      <c r="O27" s="117"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
     </row>
     <row r="28" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A28" s="70">
+      <c r="A28" s="74">
         <v>10</v>
       </c>
-      <c r="B28" s="71"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="72" t="s">
+      <c r="D28" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="73"/>
-      <c r="F28" s="71"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="75"/>
       <c r="G28" s="38">
         <v>1</v>
       </c>
@@ -2154,23 +2317,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M28" s="117"/>
-      <c r="N28" s="117"/>
-      <c r="O28" s="117"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
     </row>
     <row r="29" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A29" s="70">
+      <c r="A29" s="74">
         <v>11</v>
       </c>
-      <c r="B29" s="71"/>
+      <c r="B29" s="75"/>
       <c r="C29" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="72" t="s">
+      <c r="D29" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="73"/>
-      <c r="F29" s="71"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="75"/>
       <c r="G29" s="38">
         <v>1</v>
       </c>
@@ -2184,21 +2347,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M29" s="117"/>
-      <c r="N29" s="117"/>
-      <c r="O29" s="117"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
     </row>
     <row r="30" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A30" s="70">
+      <c r="A30" s="74">
         <v>12</v>
       </c>
-      <c r="B30" s="71"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="38"/>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="71"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="75"/>
       <c r="G30" s="38">
         <v>5</v>
       </c>
@@ -2212,21 +2375,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="117"/>
-      <c r="N30" s="117"/>
-      <c r="O30" s="117"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
     </row>
     <row r="31" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A31" s="70">
+      <c r="A31" s="74">
         <v>13</v>
       </c>
-      <c r="B31" s="71"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="38"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
+      <c r="D31" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="77"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="38">
+        <v>4</v>
+      </c>
+      <c r="H31" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="I31" s="1">
         <v>0</v>
       </c>
@@ -2234,9 +2403,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M31" s="117"/>
-      <c r="N31" s="117"/>
-      <c r="O31" s="117"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
     </row>
     <row r="32" spans="1:15" ht="23.25" thickBot="1">
       <c r="A32" s="14"/>
@@ -2256,14 +2425,14 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="22.5">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="12" t="s">
@@ -2275,14 +2444,14 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="23.25" thickBot="1">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="79"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="83"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="12" t="s">
@@ -2306,237 +2475,170 @@
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" ht="54" customHeight="1">
-      <c r="A36" s="80" t="s">
+      <c r="A36" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="80" t="s">
+      <c r="B36" s="85"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="83"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="100" t="s">
+      <c r="E36" s="87"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="101"/>
-      <c r="I36" s="101"/>
-      <c r="J36" s="102"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="103" t="s">
+      <c r="B37" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="104"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="F37" s="106"/>
-      <c r="G37" s="107" t="s">
+      <c r="E37" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="63"/>
+      <c r="G37" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="107"/>
-      <c r="I37" s="108"/>
-      <c r="J37" s="109"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="110" t="s">
+      <c r="B38" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="111"/>
+      <c r="C38" s="68"/>
       <c r="D38" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="112" t="s">
+      <c r="E38" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="113"/>
-      <c r="G38" s="114" t="s">
+      <c r="F38" s="70"/>
+      <c r="G38" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="114"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="116"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="73"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="85"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="94" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="H39" s="94"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="95"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="88"/>
-      <c r="B40" s="89"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="90"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="96"/>
-      <c r="I40" s="96"/>
-      <c r="J40" s="97"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="88"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="96"/>
-      <c r="H41" s="96"/>
-      <c r="I41" s="96"/>
-      <c r="J41" s="97"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="54"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="88"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="90"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="97"/>
+      <c r="A42" s="45"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="54"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="88"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
-      <c r="D43" s="88"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="96"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="97"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="88"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="96"/>
-      <c r="H44" s="96"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="97"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="54"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="88"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="90"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="96"/>
-      <c r="H45" s="96"/>
-      <c r="I45" s="96"/>
-      <c r="J45" s="97"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="54"/>
     </row>
     <row r="46" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A46" s="91"/>
-      <c r="B46" s="92"/>
-      <c r="C46" s="93"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="93"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="99"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="A39:C46"/>
-    <mergeCell ref="D39:F46"/>
-    <mergeCell ref="G39:J46"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:J14"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:J12"/>
@@ -2552,6 +2654,972 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="G11:J11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A39:C46"/>
+    <mergeCell ref="D39:F46"/>
+    <mergeCell ref="G39:J46"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O1048576"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="18" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="39"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="102" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A6" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" ht="66" customHeight="1">
+      <c r="A7" s="103"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" ht="22.5" customHeight="1">
+      <c r="A8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="106"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="108"/>
+    </row>
+    <row r="9" spans="1:10" ht="22.5" customHeight="1">
+      <c r="A9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="106"/>
+      <c r="I9" s="109" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="110"/>
+    </row>
+    <row r="10" spans="1:10" ht="34.5" customHeight="1">
+      <c r="A10" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="112"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="114"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A11" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="116"/>
+      <c r="C11" s="117" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="118"/>
+    </row>
+    <row r="12" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A12" s="89" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="90"/>
+      <c r="C12" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="92"/>
+    </row>
+    <row r="13" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A13" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="90"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="92"/>
+    </row>
+    <row r="14" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A14" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="90"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="92"/>
+    </row>
+    <row r="15" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A15" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="90"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="92"/>
+    </row>
+    <row r="16" spans="1:10" ht="22.5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" ht="27.75" customHeight="1">
+      <c r="A17" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="95"/>
+    </row>
+    <row r="18" spans="1:15" ht="22.5">
+      <c r="A18" s="96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="97"/>
+      <c r="C18" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="98"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A19" s="74">
+        <v>1</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="77"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="40">
+        <v>600</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="37">
+        <f>G19*I19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+    </row>
+    <row r="20" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A20" s="74">
+        <v>2</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="37">
+        <f t="shared" ref="J20:J31" si="0">G20*I20</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+    </row>
+    <row r="21" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A21" s="74">
+        <v>3</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+    </row>
+    <row r="22" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A22" s="74">
+        <v>4</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+    </row>
+    <row r="23" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A23" s="74">
+        <v>5</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+    </row>
+    <row r="24" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A24" s="74">
+        <v>6</v>
+      </c>
+      <c r="B24" s="75"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+    </row>
+    <row r="25" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A25" s="74">
+        <v>7</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+    </row>
+    <row r="26" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A26" s="74">
+        <v>8</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+    </row>
+    <row r="27" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A27" s="74">
+        <v>9</v>
+      </c>
+      <c r="B27" s="75"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+    </row>
+    <row r="28" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A28" s="74">
+        <v>10</v>
+      </c>
+      <c r="B28" s="75"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+    </row>
+    <row r="29" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A29" s="74">
+        <v>11</v>
+      </c>
+      <c r="B29" s="75"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+    </row>
+    <row r="30" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A30" s="74">
+        <v>12</v>
+      </c>
+      <c r="B30" s="75"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+    </row>
+    <row r="31" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A31" s="74">
+        <v>13</v>
+      </c>
+      <c r="B31" s="75"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+    </row>
+    <row r="32" spans="1:15" ht="23.25" thickBot="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="13">
+        <f>SUM(J19:J31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="22.5">
+      <c r="A33" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="13">
+        <f>J32*0.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="23.25" thickBot="1">
+      <c r="A34" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="13">
+        <f>SUM(J32:J33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="23.25" thickBot="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" ht="54" customHeight="1">
+      <c r="A36" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="85"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="87"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="63"/>
+      <c r="G37" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="64"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="68"/>
+      <c r="D38" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="70"/>
+      <c r="G38" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="73"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="42"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="45"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="45"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="54"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="45"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="54"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="54"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="45"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="54"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="45"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="54"/>
+    </row>
+    <row r="46" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A46" s="48"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="56"/>
+    </row>
+    <row r="1048576" spans="3:3">
+      <c r="C1048576" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="82">
+    <mergeCell ref="A39:C46"/>
+    <mergeCell ref="D39:F46"/>
+    <mergeCell ref="G39:J46"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="D5:F6"/>
+    <mergeCell ref="A6:C8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>

</xml_diff>